<commit_message>
Committing local changes before merge
</commit_message>
<xml_diff>
--- a/CheckDirectory/Financial Sample.xlsx
+++ b/CheckDirectory/Financial Sample.xlsx
@@ -617,7 +617,7 @@
         <v>19</v>
       </c>
       <c r="E2">
-        <v>1618</v>
+        <v>1818</v>
       </c>
       <c r="F2" s="1">
         <v>3</v>
@@ -1017,7 +1017,7 @@
         <v>19</v>
       </c>
       <c r="E10">
-        <v>1899</v>
+        <v>1800</v>
       </c>
       <c r="F10" s="1">
         <v>5</v>
@@ -1167,7 +1167,7 @@
         <v>19</v>
       </c>
       <c r="E13">
-        <v>2665.5</v>
+        <v>2665</v>
       </c>
       <c r="F13" s="1">
         <v>5</v>

</xml_diff>